<commit_message>
Added check for a value being an environment in .ddg.is.object.
Finished the Sivan Sampling variations with classes.
</commit_message>
<xml_diff>
--- a/examples/SivanSampling/TimingComparison.xlsx
+++ b/examples/SivanSampling/TimingComparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="100" windowWidth="18200" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>File</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Sampling-NoInstrumentation.R</t>
+  </si>
+  <si>
+    <t>Sampling-Medium.R</t>
+  </si>
+  <si>
+    <t>Sampling-Full.R</t>
   </si>
 </sst>
 </file>
@@ -578,7 +584,7 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -834,6 +840,66 @@
         <v>58</v>
       </c>
     </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.319</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.381</v>
+      </c>
+      <c r="E9" s="1">
+        <f>AVERAGE(B9:D9)</f>
+        <v>1.3433333333333335</v>
+      </c>
+      <c r="F9" s="1">
+        <v>130</v>
+      </c>
+      <c r="G9" s="1">
+        <v>93</v>
+      </c>
+      <c r="L9" s="1">
+        <v>33</v>
+      </c>
+      <c r="M9" s="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1">
+        <v>253.3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>251.9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>253</v>
+      </c>
+      <c r="E10" s="1">
+        <f>AVERAGE(B10:D10)</f>
+        <v>252.73333333333335</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4104</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3887</v>
+      </c>
+      <c r="L10" s="1">
+        <v>3116</v>
+      </c>
+      <c r="M10" s="1">
+        <v>61042</v>
+      </c>
+    </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>18</v>

</xml_diff>